<commit_message>
Created virtual environment, added requirements.txt, edited README.md
</commit_message>
<xml_diff>
--- a/result/Fiche Produit Table.xlsx
+++ b/result/Fiche Produit Table.xlsx
@@ -1,12 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Fiche Produit Table" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Fiche Produit Table" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Fiche Produit Table'!$A$1:$Y$16</definedName>
@@ -27,12 +28,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <name val="Calibri"/>
-      <family val="2"/>
       <b val="1"/>
-      <color theme="1"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -49,7 +45,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -58,33 +54,16 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
     <border>
       <left style="dotted"/>
       <right style="dotted"/>
       <top style="dotted"/>
       <bottom style="dotted"/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -95,10 +74,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -112,7 +91,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -477,7 +456,7 @@
   </sheetPr>
   <dimension ref="A1:Y16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -2613,6 +2592,6 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:Y16"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>